<commit_message>
created basic layout for spreadsheet/table
</commit_message>
<xml_diff>
--- a/Inspiration/Layout.xlsx
+++ b/Inspiration/Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b-fri\Dropbox\Private\Programming\WebDev\MyWebsite\inspiration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C978C5F-9912-4FBE-8982-63441AD8A9F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF4BE55-5B75-4FE1-8117-F8D07BD97C00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,13 +356,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,31 +653,35 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
@@ -832,10 +836,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{AE6A13C9-8B4B-4C37-BBFC-7653E1413733}"/>
-    <hyperlink ref="C13:C14" r:id="rId2" display="https://link.com" xr:uid="{1574E868-7AF7-455D-A34D-9C56A6CF9DD4}"/>
-    <hyperlink ref="C13" r:id="rId3" xr:uid="{9D4EEC83-EC89-4AAD-ABA5-9F2AB9AE46EE}"/>
-    <hyperlink ref="C14" r:id="rId4" xr:uid="{96A6611C-3A88-4509-98EA-75007B724888}"/>
+    <hyperlink ref="C14" r:id="rId1" xr:uid="{96A6611C-3A88-4509-98EA-75007B724888}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{9D4EEC83-EC89-4AAD-ABA5-9F2AB9AE46EE}"/>
+    <hyperlink ref="C13:C14" r:id="rId3" display="https://link.com" xr:uid="{1574E868-7AF7-455D-A34D-9C56A6CF9DD4}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{AE6A13C9-8B4B-4C37-BBFC-7653E1413733}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
@@ -860,10 +864,10 @@
   <sheetData>
     <row r="1" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>